<commit_message>
added cost for failures in other data results
</commit_message>
<xml_diff>
--- a/code/results/spss/other_data_caseI.xlsx
+++ b/code/results/spss/other_data_caseI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arshaali\Documents\MATLAB\artificial-trust-task-allocation\code\results\spss\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{2AAA5B37-B2B2-4C1E-8115-4627A4222B18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{848445B3-700E-42D2-8FBC-EC78E471E25F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="2835" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
   </bookViews>
   <sheets>
     <sheet name="other_data_caseI" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>ATTA Num Succ</t>
   </si>
@@ -107,6 +107,24 @@
   </si>
   <si>
     <t>Tsarouchi R Num Fail + Discarded</t>
+  </si>
+  <si>
+    <t>ATTA H Cost for Failures</t>
+  </si>
+  <si>
+    <t>ATTA R Cost for Failures</t>
+  </si>
+  <si>
+    <t>Random H Cost for Failures</t>
+  </si>
+  <si>
+    <t>Random R Cost for Failures</t>
+  </si>
+  <si>
+    <t>Tsarouchi MIN H Cost for Failures</t>
+  </si>
+  <si>
+    <t>Tsarouchi MIN R Cost for Failures</t>
   </si>
 </sst>
 </file>
@@ -947,46 +965,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC11"/>
+  <dimension ref="A1:AI11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AA5" sqref="AA5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.26953125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.08984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.6328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.54296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.453125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="29.26953125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="19.36328125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18.6328125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="29.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.36328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="28.90625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="28.7265625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="21.08984375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="23.54296875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="28.90625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="28.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1074,8 +1098,26 @@
       <c r="AC1" t="s">
         <v>28</v>
       </c>
+      <c r="AD1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>410</v>
       </c>
@@ -1163,8 +1205,26 @@
       <c r="AC2">
         <v>49</v>
       </c>
+      <c r="AD2">
+        <v>2.0843366441311799</v>
+      </c>
+      <c r="AE2">
+        <v>11.3005853723268</v>
+      </c>
+      <c r="AF2">
+        <v>16.432125115786501</v>
+      </c>
+      <c r="AG2">
+        <v>12.559642086380199</v>
+      </c>
+      <c r="AH2">
+        <v>9.3898869019654594</v>
+      </c>
+      <c r="AI2">
+        <v>3.9959030524759398</v>
+      </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>392</v>
       </c>
@@ -1252,8 +1312,26 @@
       <c r="AC3">
         <v>58</v>
       </c>
+      <c r="AD3">
+        <v>1.33725748000518</v>
+      </c>
+      <c r="AE3">
+        <v>14.3335699508559</v>
+      </c>
+      <c r="AF3">
+        <v>21.722011581827299</v>
+      </c>
+      <c r="AG3">
+        <v>12.889650581358801</v>
+      </c>
+      <c r="AH3">
+        <v>10.2739830714657</v>
+      </c>
+      <c r="AI3">
+        <v>4.7325541979824903</v>
+      </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>395</v>
       </c>
@@ -1341,8 +1419,26 @@
       <c r="AC4">
         <v>54</v>
       </c>
+      <c r="AD4">
+        <v>2.3566511075727701</v>
+      </c>
+      <c r="AE4">
+        <v>13.658935975225599</v>
+      </c>
+      <c r="AF4">
+        <v>19.8765132676115</v>
+      </c>
+      <c r="AG4">
+        <v>13.3454528397969</v>
+      </c>
+      <c r="AH4">
+        <v>11.2566146279178</v>
+      </c>
+      <c r="AI4">
+        <v>4.5002690207741001</v>
+      </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>397</v>
       </c>
@@ -1430,8 +1526,26 @@
       <c r="AC5">
         <v>59</v>
       </c>
+      <c r="AD5">
+        <v>2.0798293450997001</v>
+      </c>
+      <c r="AE5">
+        <v>13.178863475239</v>
+      </c>
+      <c r="AF5">
+        <v>22.815951038125299</v>
+      </c>
+      <c r="AG5">
+        <v>14.209063805568301</v>
+      </c>
+      <c r="AH5">
+        <v>12.204985795034499</v>
+      </c>
+      <c r="AI5">
+        <v>4.9240618668343901</v>
+      </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>400</v>
       </c>
@@ -1519,8 +1633,26 @@
       <c r="AC6">
         <v>52</v>
       </c>
+      <c r="AD6">
+        <v>0.82330166017134998</v>
+      </c>
+      <c r="AE6">
+        <v>13.479453889128299</v>
+      </c>
+      <c r="AF6">
+        <v>23.0478389263879</v>
+      </c>
+      <c r="AG6">
+        <v>11.3044702886891</v>
+      </c>
+      <c r="AH6">
+        <v>12.8660490073537</v>
+      </c>
+      <c r="AI6">
+        <v>4.3606936753822696</v>
+      </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>405</v>
       </c>
@@ -1608,8 +1740,26 @@
       <c r="AC7">
         <v>52</v>
       </c>
+      <c r="AD7">
+        <v>1.93700779548671</v>
+      </c>
+      <c r="AE7">
+        <v>12.4772936183819</v>
+      </c>
+      <c r="AF7">
+        <v>23.020128270590899</v>
+      </c>
+      <c r="AG7">
+        <v>11.630967747175299</v>
+      </c>
+      <c r="AH7">
+        <v>10.431218249683001</v>
+      </c>
+      <c r="AI7">
+        <v>4.2552139952902799</v>
+      </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>392</v>
       </c>
@@ -1697,8 +1847,26 @@
       <c r="AC8">
         <v>55</v>
       </c>
+      <c r="AD8">
+        <v>1.2758997942449699</v>
+      </c>
+      <c r="AE8">
+        <v>14.049310205823399</v>
+      </c>
+      <c r="AF8">
+        <v>19.923239031373701</v>
+      </c>
+      <c r="AG8">
+        <v>13.260277285523101</v>
+      </c>
+      <c r="AH8">
+        <v>13.148432820491999</v>
+      </c>
+      <c r="AI8">
+        <v>4.5391094966868897</v>
+      </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>384</v>
       </c>
@@ -1786,8 +1954,26 @@
       <c r="AC9">
         <v>60</v>
       </c>
+      <c r="AD9">
+        <v>1.35007971880422</v>
+      </c>
+      <c r="AE9">
+        <v>15.092534410311201</v>
+      </c>
+      <c r="AF9">
+        <v>23.6100964275333</v>
+      </c>
+      <c r="AG9">
+        <v>13.4076155817519</v>
+      </c>
+      <c r="AH9">
+        <v>11.987769179998899</v>
+      </c>
+      <c r="AI9">
+        <v>4.9435165177143201</v>
+      </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>410</v>
       </c>
@@ -1875,8 +2061,26 @@
       <c r="AC10">
         <v>56</v>
       </c>
+      <c r="AD10">
+        <v>2.3816939623441198</v>
+      </c>
+      <c r="AE10">
+        <v>12.0065924121413</v>
+      </c>
+      <c r="AF10">
+        <v>18.175618560538499</v>
+      </c>
+      <c r="AG10">
+        <v>11.1517607286002</v>
+      </c>
+      <c r="AH10">
+        <v>9.9595832081362108</v>
+      </c>
+      <c r="AI10">
+        <v>4.5272965123244502</v>
+      </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>399</v>
       </c>
@@ -1963,6 +2167,24 @@
       </c>
       <c r="AC11">
         <v>57</v>
+      </c>
+      <c r="AD11">
+        <v>0.65111910368157</v>
+      </c>
+      <c r="AE11">
+        <v>14.149850474089799</v>
+      </c>
+      <c r="AF11">
+        <v>24.371990196236901</v>
+      </c>
+      <c r="AG11">
+        <v>12.743832954299799</v>
+      </c>
+      <c r="AH11">
+        <v>11.0711078085212</v>
+      </c>
+      <c r="AI11">
+        <v>4.6526274827717504</v>
       </c>
     </row>
   </sheetData>

</xml_diff>